<commit_message>
Author        :Prateek Kapoor Story ID      :SSDMS 36 Task          : Story Deleted Description   : Story ID SSDMS 36 Deleted because it was not a requirement
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/Backlog/Backlog.xlsx
+++ b/SSDMS_Requirements/Backlog/Backlog.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="154">
   <si>
     <t>Epic</t>
   </si>
@@ -281,9 +281,6 @@
     <t xml:space="preserve">As a product owner, I want backend logic (High Charts) to be integrated so that Infographic -4 is displayed with real time information </t>
   </si>
   <si>
-    <t>As a product owner, I want date filter to be configured for the page so that the charts are updated based on selected filter criteria</t>
-  </si>
-  <si>
     <t>SSDMS-27</t>
   </si>
   <si>
@@ -329,9 +326,6 @@
     <t>As a product owner, I want comments to be entered for an application so that those are visible to the applicant for correcting the application.</t>
   </si>
   <si>
-    <t>SSDMS-36</t>
-  </si>
-  <si>
     <t>SSDMS-37</t>
   </si>
   <si>
@@ -531,24 +525,6 @@
   </si>
   <si>
     <t>As a product owner, I want Reset button option on the page, so that user can reset the type of user role.</t>
-  </si>
-  <si>
-    <t>Pooja Sharma</t>
-  </si>
-  <si>
-    <t>Alkesh</t>
-  </si>
-  <si>
-    <t>Deepak Kandpal</t>
-  </si>
-  <si>
-    <t>Ashish Mishra</t>
-  </si>
-  <si>
-    <t>Ekansh Kumar</t>
-  </si>
-  <si>
-    <t>Bhanu P Tiwari</t>
   </si>
 </sst>
 </file>
@@ -1167,11 +1143,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,10 +1174,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1221,7 +1197,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="13"/>
     </row>
@@ -1232,10 +1208,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F3" s="13"/>
     </row>
@@ -1249,7 +1225,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F4" s="13"/>
     </row>
@@ -1263,7 +1239,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F5" s="13"/>
     </row>
@@ -1277,7 +1253,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F6" s="13"/>
     </row>
@@ -1290,10 +1266,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F7" s="13"/>
     </row>
@@ -1304,10 +1280,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F8" s="13"/>
     </row>
@@ -1321,7 +1297,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F9" s="13"/>
     </row>
@@ -1335,7 +1311,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F10" s="13"/>
     </row>
@@ -1349,7 +1325,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F11" s="13"/>
     </row>
@@ -1367,7 +1343,7 @@
         <v>32</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F12" s="13"/>
     </row>
@@ -1381,7 +1357,7 @@
         <v>33</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F13" s="13"/>
     </row>
@@ -1395,7 +1371,7 @@
         <v>34</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F14" s="13"/>
     </row>
@@ -1409,7 +1385,7 @@
         <v>37</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="13"/>
     </row>
@@ -1423,7 +1399,7 @@
         <v>36</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F16" s="13"/>
     </row>
@@ -1431,13 +1407,13 @@
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>151</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="1"/>
@@ -1456,7 +1432,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F18" s="13"/>
     </row>
@@ -1470,7 +1446,7 @@
         <v>40</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F19" s="13"/>
     </row>
@@ -1484,7 +1460,7 @@
         <v>41</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F20" s="13"/>
     </row>
@@ -1498,7 +1474,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F21" s="13"/>
     </row>
@@ -1509,10 +1485,10 @@
         <v>44</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F22" s="13"/>
     </row>
@@ -1526,7 +1502,7 @@
         <v>43</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F23" s="13"/>
     </row>
@@ -1540,7 +1516,7 @@
         <v>45</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F24" s="13"/>
     </row>
@@ -1554,7 +1530,7 @@
         <v>46</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F25" s="13"/>
     </row>
@@ -1572,7 +1548,7 @@
         <v>54</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F26" s="13"/>
     </row>
@@ -1586,7 +1562,7 @@
         <v>55</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F27" s="13"/>
     </row>
@@ -1600,7 +1576,7 @@
         <v>56</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F28" s="13"/>
     </row>
@@ -1614,7 +1590,7 @@
         <v>58</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F29" s="13"/>
     </row>
@@ -1622,13 +1598,13 @@
       <c r="A30" s="22"/>
       <c r="B30" s="22"/>
       <c r="C30" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F30" s="13"/>
     </row>
@@ -1640,13 +1616,13 @@
         <v>64</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F31" s="13"/>
     </row>
@@ -1654,13 +1630,13 @@
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
       <c r="C32" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>66</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F32" s="13"/>
     </row>
@@ -1668,13 +1644,13 @@
       <c r="A33" s="22"/>
       <c r="B33" s="22"/>
       <c r="C33" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F33" s="13"/>
     </row>
@@ -1682,13 +1658,13 @@
       <c r="A34" s="22"/>
       <c r="B34" s="22"/>
       <c r="C34" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F34" s="13"/>
     </row>
@@ -1696,13 +1672,13 @@
       <c r="A35" s="22"/>
       <c r="B35" s="22"/>
       <c r="C35" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F35" s="13"/>
     </row>
@@ -1710,13 +1686,13 @@
       <c r="A36" s="22"/>
       <c r="B36" s="22"/>
       <c r="C36" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>69</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F36" s="13"/>
     </row>
@@ -1724,13 +1700,13 @@
       <c r="A37" s="22"/>
       <c r="B37" s="22"/>
       <c r="C37" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>70</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F37" s="13"/>
     </row>
@@ -1738,143 +1714,129 @@
       <c r="A38" s="22"/>
       <c r="B38" s="22"/>
       <c r="C38" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>71</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="9" t="s">
-        <v>88</v>
+      <c r="B39" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>134</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E39" s="19"/>
       <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="23" t="s">
-        <v>82</v>
-      </c>
+      <c r="B40" s="24"/>
       <c r="C40" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>156</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E40" s="19"/>
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="22"/>
       <c r="B41" s="24"/>
       <c r="C41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>157</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E41" s="19"/>
       <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
       <c r="B42" s="24"/>
       <c r="C42" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="19" t="s">
-        <v>158</v>
-      </c>
+      <c r="E42" s="19"/>
       <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
       <c r="B43" s="24"/>
       <c r="C43" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="19" t="s">
-        <v>158</v>
-      </c>
+      <c r="E43" s="19"/>
       <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
       <c r="B44" s="24"/>
       <c r="C44" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="19" t="s">
-        <v>157</v>
-      </c>
+      <c r="E44" s="19"/>
       <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="24"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>159</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="E45" s="19"/>
       <c r="F45" s="13"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="3" t="s">
-        <v>100</v>
+      <c r="B46" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>99</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="F46" s="13"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="22" t="s">
-        <v>94</v>
-      </c>
+      <c r="B47" s="22"/>
       <c r="C47" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F47" s="13"/>
     </row>
@@ -1882,13 +1844,13 @@
       <c r="A48" s="22"/>
       <c r="B48" s="22"/>
       <c r="C48" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F48" s="13"/>
     </row>
@@ -1896,13 +1858,13 @@
       <c r="A49" s="22"/>
       <c r="B49" s="22"/>
       <c r="C49" s="10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F49" s="13"/>
     </row>
@@ -1910,43 +1872,43 @@
       <c r="A50" s="22"/>
       <c r="B50" s="22"/>
       <c r="C50" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F50" s="13"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="10" t="s">
-        <v>109</v>
+      <c r="B51" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="22"/>
-      <c r="B52" s="22" t="s">
-        <v>104</v>
-      </c>
+      <c r="B52" s="22"/>
       <c r="C52" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F52" s="13"/>
     </row>
@@ -1954,13 +1916,13 @@
       <c r="A53" s="22"/>
       <c r="B53" s="22"/>
       <c r="C53" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D53" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F53" s="13"/>
     </row>
@@ -1968,115 +1930,89 @@
       <c r="A54" s="22"/>
       <c r="B54" s="22"/>
       <c r="C54" s="8" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F54" s="13"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="8" t="s">
-        <v>123</v>
+      <c r="B55" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>138</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E55" s="19"/>
       <c r="F55" s="13"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="22"/>
-      <c r="B56" s="22" t="s">
-        <v>112</v>
-      </c>
+      <c r="B56" s="22"/>
       <c r="C56" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>157</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E56" s="19"/>
       <c r="F56" s="13"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
       <c r="B57" s="22"/>
       <c r="C57" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>160</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E57" s="19"/>
       <c r="F57" s="13"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="22"/>
       <c r="B58" s="22"/>
       <c r="C58" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>156</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E58" s="19"/>
       <c r="F58" s="13"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
       <c r="B59" s="22"/>
       <c r="C59" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>160</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E59" s="19"/>
       <c r="F59" s="13"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
       <c r="B60" s="22"/>
       <c r="C60" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>159</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E60" s="19"/>
       <c r="F60" s="13"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="F61" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2085,16 +2021,16 @@
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B12:B17"/>
     <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="A31:A61"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="A31:A60"/>
     <mergeCell ref="B18:B25"/>
     <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="B51:B54"/>
     <mergeCell ref="B26:B30"/>
     <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="B40:B46"/>
+    <mergeCell ref="B31:B38"/>
+    <mergeCell ref="B39:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
@@ -2126,10 +2062,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Author       : Priyanshu Pandey Description  : Stories+ Backlogs
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/Backlog/Backlog.xlsx
+++ b/SSDMS_Requirements/Backlog/Backlog.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="179">
   <si>
     <t>Epic</t>
   </si>
@@ -281,6 +281,9 @@
     <t xml:space="preserve">As a product owner, I want backend logic (High Charts) to be integrated so that Infographic -4 is displayed with real time information </t>
   </si>
   <si>
+    <t>As a product owner, I want date filter to be configured for the page so that the charts are updated based on selected filter criteria</t>
+  </si>
+  <si>
     <t>SSDMS-27</t>
   </si>
   <si>
@@ -326,6 +329,9 @@
     <t>As a product owner, I want comments to be entered for an application so that those are visible to the applicant for correcting the application.</t>
   </si>
   <si>
+    <t>SSDMS-36</t>
+  </si>
+  <si>
     <t>SSDMS-37</t>
   </si>
   <si>
@@ -525,12 +531,81 @@
   </si>
   <si>
     <t>As a product owner, I want Reset button option on the page, so that user can reset the type of user role.</t>
+  </si>
+  <si>
+    <t>Pooja Sharma</t>
+  </si>
+  <si>
+    <t>Alkesh</t>
+  </si>
+  <si>
+    <t>Deepak Kandpal</t>
+  </si>
+  <si>
+    <t>Ashish Mishra</t>
+  </si>
+  <si>
+    <t>Ekansh Kumar</t>
+  </si>
+  <si>
+    <t>Bhanu P Tiwari</t>
+  </si>
+  <si>
+    <t>Homepage AB</t>
+  </si>
+  <si>
+    <t>SSDMS-59</t>
+  </si>
+  <si>
+    <t>SSDMS-60</t>
+  </si>
+  <si>
+    <t>SSDMS-61</t>
+  </si>
+  <si>
+    <t>SSDMS-62</t>
+  </si>
+  <si>
+    <t>SSDMS-63</t>
+  </si>
+  <si>
+    <t>Homepage TP</t>
+  </si>
+  <si>
+    <t>As a product owner, I want 'Result status' option so that assessment body can notify that the results of candidates have been uploaded or not</t>
+  </si>
+  <si>
+    <t>As a product owner, I want an 'Add Centre' option on the page so that TP can add new centre</t>
+  </si>
+  <si>
+    <t>As a product owner, I want a 'download certificate' option so that TP can download certificates of their batch(es)</t>
+  </si>
+  <si>
+    <t>As a product owner, I want a 'download invoice' option so that TP can download fee invoices of their batch(es)</t>
+  </si>
+  <si>
+    <t>As a product owner, I want 'assessment status' option so that Assessment body can notify about the assessment status of the candidates</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>SSDMS-64</t>
+  </si>
+  <si>
+    <t>SSDMS-65</t>
+  </si>
+  <si>
+    <t>As a product owner, I want an 'Import Certificate' option so that I can upload the certificate of assessed candidates</t>
+  </si>
+  <si>
+    <t>As a product owner, I want a 'download' option so that I can download the result of FAQs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,7 +648,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -637,6 +712,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -772,6 +853,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -780,6 +864,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1143,11 +1232,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,20 +1263,20 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1197,27 +1286,27 @@
         <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1225,13 +1314,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1239,13 +1328,13 @@
         <v>20</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1253,43 +1342,43 @@
         <v>21</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1297,13 +1386,13 @@
         <v>22</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1311,13 +1400,13 @@
         <v>35</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1325,15 +1414,15 @@
         <v>20</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1343,13 +1432,13 @@
         <v>32</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1357,13 +1446,13 @@
         <v>33</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1371,13 +1460,13 @@
         <v>34</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
@@ -1385,13 +1474,13 @@
         <v>37</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
@@ -1399,30 +1488,30 @@
         <v>36</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1432,13 +1521,13 @@
         <v>39</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="5" t="s">
         <v>29</v>
       </c>
@@ -1446,13 +1535,13 @@
         <v>40</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="5" t="s">
         <v>30</v>
       </c>
@@ -1460,13 +1549,13 @@
         <v>41</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="5" t="s">
         <v>31</v>
       </c>
@@ -1474,27 +1563,27 @@
         <v>42</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1502,13 +1591,13 @@
         <v>43</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
@@ -1516,13 +1605,13 @@
         <v>45</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1530,15 +1619,15 @@
         <v>46</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="23" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -1548,13 +1637,13 @@
         <v>54</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="6" t="s">
         <v>52</v>
       </c>
@@ -1562,13 +1651,13 @@
         <v>55</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="6" t="s">
         <v>53</v>
       </c>
@@ -1576,13 +1665,13 @@
         <v>56</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="6" t="s">
         <v>57</v>
       </c>
@@ -1590,447 +1679,560 @@
         <v>58</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="23" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>66</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D34" s="16" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>69</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>70</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
       <c r="C38" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>71</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>87</v>
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D39" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="13"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="24"/>
       <c r="C40" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E40" s="19"/>
+        <v>83</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>156</v>
+      </c>
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="24"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E41" s="19"/>
+        <v>118</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="19"/>
+      <c r="E42" s="19" t="s">
+        <v>158</v>
+      </c>
       <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="24"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D43" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="19"/>
+      <c r="E43" s="19" t="s">
+        <v>158</v>
+      </c>
       <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D44" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="19"/>
+      <c r="E44" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="25"/>
       <c r="C45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F48" s="13"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="E51" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F53" s="13"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="23"/>
+      <c r="C54" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F57" s="13"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="13"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F46" s="13"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="F47" s="13"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="F48" s="13"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="F49" s="13"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="F50" s="13"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="F52" s="13"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D53" s="16" t="s">
+      <c r="D59" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F60" s="13"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="F61" s="13"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="23"/>
+      <c r="C63" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="23"/>
+      <c r="C65" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="23"/>
+      <c r="C66" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C67" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="F53" s="13"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="F54" s="13"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E55" s="19"/>
-      <c r="F55" s="13"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E56" s="19"/>
-      <c r="F56" s="13"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="13"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="22"/>
-      <c r="C58" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E58" s="19"/>
-      <c r="F58" s="13"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E59" s="19"/>
-      <c r="F59" s="13"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" s="19"/>
-      <c r="F60" s="13"/>
+      <c r="C68" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="A31:A61"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="B40:B46"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B12:B17"/>
     <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="A31:A60"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B31:B38"/>
-    <mergeCell ref="B39:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
@@ -2062,10 +2264,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Author      : Priyanshu Pandey Description : Stories+Backlogs
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/Backlog/Backlog.xlsx
+++ b/SSDMS_Requirements/Backlog/Backlog.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="179">
   <si>
     <t>Epic</t>
   </si>
@@ -813,7 +813,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -853,6 +853,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -865,10 +870,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1234,9 +1237,9 @@
   </sheetPr>
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,10 +1276,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1291,8 +1294,8 @@
       <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1305,8 +1308,8 @@
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1319,8 +1322,8 @@
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1333,8 +1336,8 @@
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1347,8 +1350,8 @@
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -1363,8 +1366,8 @@
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1377,8 +1380,8 @@
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1391,8 +1394,8 @@
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
@@ -1405,8 +1408,8 @@
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1419,10 +1422,10 @@
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="27" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -1437,8 +1440,8 @@
       <c r="F12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1451,8 +1454,8 @@
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
@@ -1465,8 +1468,8 @@
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
@@ -1479,8 +1482,8 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
@@ -1493,8 +1496,8 @@
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="8" t="s">
         <v>149</v>
       </c>
@@ -1508,10 +1511,10 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1526,8 +1529,8 @@
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="5" t="s">
         <v>29</v>
       </c>
@@ -1540,8 +1543,8 @@
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="5" t="s">
         <v>30</v>
       </c>
@@ -1554,8 +1557,8 @@
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
       <c r="C21" s="5" t="s">
         <v>31</v>
       </c>
@@ -1568,8 +1571,8 @@
       <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
@@ -1582,8 +1585,8 @@
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="5" t="s">
         <v>47</v>
       </c>
@@ -1596,8 +1599,8 @@
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
@@ -1610,8 +1613,8 @@
       <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="5" t="s">
         <v>50</v>
       </c>
@@ -1624,10 +1627,10 @@
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="26" t="s">
         <v>49</v>
       </c>
       <c r="C26" s="6" t="s">
@@ -1642,8 +1645,8 @@
       <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="6" t="s">
         <v>52</v>
       </c>
@@ -1656,8 +1659,8 @@
       <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="6" t="s">
         <v>53</v>
       </c>
@@ -1670,8 +1673,8 @@
       <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="6" t="s">
         <v>57</v>
       </c>
@@ -1684,8 +1687,8 @@
       <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="6" t="s">
         <v>73</v>
       </c>
@@ -1698,10 +1701,10 @@
       <c r="F30" s="13"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="26" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -1716,8 +1719,8 @@
       <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="9" t="s">
         <v>75</v>
       </c>
@@ -1730,8 +1733,8 @@
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="9" t="s">
         <v>76</v>
       </c>
@@ -1744,8 +1747,8 @@
       <c r="F33" s="13"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="9" t="s">
         <v>77</v>
       </c>
@@ -1758,8 +1761,8 @@
       <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="9" t="s">
         <v>78</v>
       </c>
@@ -1772,8 +1775,8 @@
       <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="9" t="s">
         <v>79</v>
       </c>
@@ -1786,8 +1789,8 @@
       <c r="F36" s="13"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="9" t="s">
         <v>80</v>
       </c>
@@ -1800,8 +1803,8 @@
       <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="9" t="s">
         <v>81</v>
       </c>
@@ -1814,8 +1817,8 @@
       <c r="F38" s="13"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="9" t="s">
         <v>88</v>
       </c>
@@ -1828,8 +1831,8 @@
       <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="27" t="s">
         <v>82</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -1844,8 +1847,8 @@
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="3" t="s">
         <v>90</v>
       </c>
@@ -1858,8 +1861,8 @@
       <c r="F41" s="13"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="25"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="3" t="s">
         <v>91</v>
       </c>
@@ -1872,8 +1875,8 @@
       <c r="F42" s="13"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
-      <c r="B43" s="25"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="3" t="s">
         <v>92</v>
       </c>
@@ -1886,8 +1889,8 @@
       <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="25"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="3" t="s">
         <v>93</v>
       </c>
@@ -1900,8 +1903,8 @@
       <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="3" t="s">
         <v>99</v>
       </c>
@@ -1914,8 +1917,8 @@
       <c r="F45" s="13"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="29"/>
       <c r="C46" s="3" t="s">
         <v>100</v>
       </c>
@@ -1928,8 +1931,8 @@
       <c r="F46" s="13"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23" t="s">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -1944,8 +1947,8 @@
       <c r="F47" s="13"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="23"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
       <c r="C48" s="10" t="s">
         <v>102</v>
       </c>
@@ -1958,8 +1961,8 @@
       <c r="F48" s="13"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="10" t="s">
         <v>103</v>
       </c>
@@ -1972,8 +1975,8 @@
       <c r="F49" s="13"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="23"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="10" t="s">
         <v>108</v>
       </c>
@@ -1986,8 +1989,8 @@
       <c r="F50" s="13"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="10" t="s">
         <v>109</v>
       </c>
@@ -2000,8 +2003,8 @@
       <c r="F51" s="13"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="23" t="s">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26" t="s">
         <v>104</v>
       </c>
       <c r="C52" s="8" t="s">
@@ -2016,8 +2019,8 @@
       <c r="F52" s="13"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="23"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="8" t="s">
         <v>111</v>
       </c>
@@ -2030,8 +2033,8 @@
       <c r="F53" s="13"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
       <c r="C54" s="8" t="s">
         <v>116</v>
       </c>
@@ -2044,8 +2047,8 @@
       <c r="F54" s="13"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="8" t="s">
         <v>123</v>
       </c>
@@ -2058,8 +2061,8 @@
       <c r="F55" s="13"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="23" t="s">
+      <c r="A56" s="26"/>
+      <c r="B56" s="26" t="s">
         <v>112</v>
       </c>
       <c r="C56" s="11" t="s">
@@ -2074,8 +2077,8 @@
       <c r="F56" s="13"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="23"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="11" t="s">
         <v>125</v>
       </c>
@@ -2088,8 +2091,8 @@
       <c r="F57" s="13"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="11" t="s">
         <v>126</v>
       </c>
@@ -2102,8 +2105,8 @@
       <c r="F58" s="13"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="11" t="s">
         <v>127</v>
       </c>
@@ -2116,8 +2119,8 @@
       <c r="F59" s="13"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
       <c r="C60" s="11" t="s">
         <v>130</v>
       </c>
@@ -2130,8 +2133,8 @@
       <c r="F60" s="13"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="23"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="11" t="s">
         <v>131</v>
       </c>
@@ -2144,78 +2147,104 @@
       <c r="F61" s="13"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="C62" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="24" t="s">
         <v>173</v>
       </c>
+      <c r="E62" s="30" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
-      <c r="C63" s="27" t="s">
+      <c r="B63" s="26"/>
+      <c r="C63" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="D63" s="28" t="s">
+      <c r="D63" s="24" t="s">
         <v>169</v>
       </c>
+      <c r="E63" s="30" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="23" t="s">
+      <c r="B64" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="C64" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="D64" s="28" t="s">
+      <c r="D64" s="24" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="23"/>
-      <c r="C65" s="27" t="s">
+      <c r="E64" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="26"/>
+      <c r="C65" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="D65" s="28" t="s">
+      <c r="D65" s="24" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="23"/>
-      <c r="C66" s="27" t="s">
+      <c r="E65" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="26"/>
+      <c r="C66" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D66" s="28" t="s">
+      <c r="D66" s="24" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C67" s="23" t="s">
         <v>175</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="29" t="s">
+      <c r="E67" s="30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C68" s="27" t="s">
+      <c r="C68" s="23" t="s">
         <v>176</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="E68" s="30" t="s">
+        <v>142</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="A12:A17"/>
     <mergeCell ref="B62:B63"/>
     <mergeCell ref="B64:B66"/>
     <mergeCell ref="B56:B61"/>
@@ -2228,11 +2257,6 @@
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="B31:B39"/>
     <mergeCell ref="B40:B46"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="A12:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Author: Pravek Saxena Description: Renamed a duplicate story with ID SSDMS 11 to SSDMS 11'
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/Backlog/Backlog.xlsx
+++ b/SSDMS_Requirements/Backlog/Backlog.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="164">
   <si>
     <t>Epic</t>
   </si>
@@ -552,6 +552,9 @@
   </si>
   <si>
     <t>As a product owner, I want HTML and CSS to be created for the page so that necessary skeleton is developed for the page as per GD and adding comment box</t>
+  </si>
+  <si>
+    <t>SSDMS-11'</t>
   </si>
 </sst>
 </file>
@@ -1172,9 +1175,9 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,7 +1381,7 @@
       <c r="A13" s="24"/>
       <c r="B13" s="24"/>
       <c r="C13" s="8" t="s">
-        <v>17</v>
+        <v>163</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>33</v>
@@ -2083,6 +2086,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="A12:A17"/>
     <mergeCell ref="B56:B61"/>
     <mergeCell ref="A31:A61"/>
     <mergeCell ref="B18:B25"/>
@@ -2093,11 +2101,6 @@
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="B31:B39"/>
     <mergeCell ref="B40:B46"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="A12:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Author     : Priyanshu Pandey Story ID   : SSDMS-17 Task       : Story deleted Description: SSDMS-17 was deleted because it was of no use
Story ID   : SSDMS-59 to SSDMS-65
Task       : Backlog stories added
Description: Backlog stories were added at the end of document
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/Backlog/Backlog.xlsx
+++ b/SSDMS_Requirements/Backlog/Backlog.xlsx
@@ -20,7 +20,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D22" authorId="0" shapeId="0">
+    <comment ref="D21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="0" shapeId="0">
+    <comment ref="D31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="177">
   <si>
     <t>Epic</t>
   </si>
@@ -152,9 +152,6 @@
     <t>SSDMS-15</t>
   </si>
   <si>
-    <t>SSDMS-16</t>
-  </si>
-  <si>
     <t>SSDMS-17</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>As a product owner, I want HTML with CSS to be created for all scenarios of AB homepage so that page looks as agreed in the GD</t>
   </si>
   <si>
-    <t>As a product owner, I want present batches information to be displayed so that AB can see the existing batches information on their landing page</t>
-  </si>
-  <si>
     <t>As a product owner, I want past batches information to be displayed so that AB can see the old batches information on their landing page</t>
   </si>
   <si>
@@ -551,16 +545,61 @@
     <t>Bhanu P Tiwari</t>
   </si>
   <si>
-    <t>As a product owner, I want HTML and CSS to be created for the page so that necessary skeleton is developed for the page as per GD and adding comment box</t>
-  </si>
-  <si>
-    <t>SSDMS-11'</t>
+    <t>Homepage AB</t>
+  </si>
+  <si>
+    <t>SSDMS-59</t>
+  </si>
+  <si>
+    <t>SSDMS-60</t>
+  </si>
+  <si>
+    <t>SSDMS-61</t>
+  </si>
+  <si>
+    <t>SSDMS-62</t>
+  </si>
+  <si>
+    <t>SSDMS-63</t>
+  </si>
+  <si>
+    <t>Homepage TP</t>
+  </si>
+  <si>
+    <t>As a product owner, I want 'Result status' option so that assessment body can notify that the results of candidates have been uploaded or not</t>
+  </si>
+  <si>
+    <t>As a product owner, I want an 'Add Centre' option on the page so that TP can add new centre</t>
+  </si>
+  <si>
+    <t>As a product owner, I want a 'download certificate' option so that TP can download certificates of their batch(es)</t>
+  </si>
+  <si>
+    <t>As a product owner, I want a 'download invoice' option so that TP can download fee invoices of their batch(es)</t>
+  </si>
+  <si>
+    <t>As a product owner, I want 'assessment status' option so that Assessment body can notify about the assessment status of the candidates</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>SSDMS-64</t>
+  </si>
+  <si>
+    <t>SSDMS-65</t>
+  </si>
+  <si>
+    <t>As a product owner, I want an 'Import Certificate' option so that I can upload the certificate of assessed candidates</t>
+  </si>
+  <si>
+    <t>As a product owner, I want a 'download' option so that I can download the result of FAQs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,7 +642,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -667,6 +706,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -797,6 +842,17 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1173,11 +1229,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,20 +1260,20 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1227,27 +1283,27 @@
         <v>18</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1255,13 +1311,13 @@
         <v>19</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1269,13 +1325,13 @@
         <v>20</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1283,43 +1339,43 @@
         <v>21</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1327,27 +1383,27 @@
         <v>22</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1355,178 +1411,178 @@
         <v>20</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>61</v>
+      <c r="B12" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="E13" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="8" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>151</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>38</v>
+      <c r="A18" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>115</v>
-      </c>
       <c r="E22" s="19" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>43</v>
@@ -1537,13 +1593,13 @@
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>146</v>
@@ -1551,73 +1607,73 @@
       <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="5" t="s">
+      <c r="A25" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D27" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="E27" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>56</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="E29" s="19" t="s">
         <v>146</v>
@@ -1625,73 +1681,73 @@
       <c r="F29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="6" t="s">
+      <c r="A30" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="22" t="s">
+      <c r="D31" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="E31" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D32" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="13"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="16" t="s">
+      <c r="E33" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>66</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="13"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>67</v>
       </c>
       <c r="E34" s="20" t="s">
         <v>135</v>
@@ -1699,141 +1755,141 @@
       <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D36" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F35" s="13"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="9" t="s">
+      <c r="E36" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F36" s="13"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D37" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F36" s="13"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="9" t="s">
+      <c r="E37" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="27"/>
+      <c r="B39" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F37" s="13"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F38" s="13"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="9" t="s">
+      <c r="E39" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="27"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F39" s="13"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23" t="s">
+      <c r="D40" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="27"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="16" t="s">
+      <c r="E41" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="27"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E42" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="F40" s="13"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" s="13"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="3" t="s">
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D43" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E42" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="F42" s="13"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="16" t="s">
+      <c r="E43" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="27"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="F43" s="13"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="E44" s="19" t="s">
         <v>157</v>
@@ -1841,229 +1897,229 @@
       <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="27"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="F45" s="13"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D47" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="13"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="27"/>
+      <c r="B51" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53" s="13"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57" s="13"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F58" s="13"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F59" s="13"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E46" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="F46" s="13"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="F47" s="13"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="F48" s="13"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="F49" s="13"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F50" s="13"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="F51" s="13"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="F52" s="13"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-      <c r="C53" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="F53" s="13"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="F54" s="13"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
-      <c r="C55" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="F55" s="13"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="22"/>
-      <c r="B56" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="D56" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F56" s="13"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="F57" s="13"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
-      <c r="B58" s="22"/>
-      <c r="C58" s="11" t="s">
+      <c r="D60" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="D58" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="F58" s="13"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="F59" s="13"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>122</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>159</v>
@@ -2071,36 +2127,116 @@
       <c r="F60" s="13"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="D61" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E61" s="19" t="s">
+      <c r="B61" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F61" s="13"/>
+      <c r="D61" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="E61" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="27"/>
+      <c r="C62" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="27"/>
+      <c r="C64" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="27"/>
+      <c r="C65" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B65"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="A30:A60"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="B39:B45"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B12:B17"/>
     <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="A31:A61"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="A18:A25"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="B40:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
@@ -2132,10 +2268,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>

</xml_diff>